<commit_message>
Catch import file format errors
</commit_message>
<xml_diff>
--- a/src/reviews/tests/fixtures/distrib_list_unknown_user.xlsx
+++ b/src/reviews/tests/fixtures/distrib_list_unknown_user.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>user1@test.com</t>
   </si>
@@ -161,7 +161,7 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -169,7 +169,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="6" min="2" style="0" width="3.64372469635628"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -219,9 +219,6 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>